<commit_message>
:sparkles: model last columns in template import
* parse image timedelta string
* insert physiological and developmental stage
</commit_message>
<xml_diff>
--- a/django-data/image/common/tests/Image_sample_template_with_example_20190405.xlsx
+++ b/django-data/image/common/tests/Image_sample_template_with_example_20190405.xlsx
@@ -1,18 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Paolo\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92159F0-2DAE-4B3A-9A22-617E983908AC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="sheetColumnCount" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="ontology" sheetId="2" r:id="rId4"/>
-    <sheet state="visible" name="submission" sheetId="3" r:id="rId5"/>
-    <sheet state="visible" name="contact" sheetId="4" r:id="rId6"/>
-    <sheet state="visible" name="breed" sheetId="5" r:id="rId7"/>
-    <sheet state="visible" name="animal" sheetId="6" r:id="rId8"/>
-    <sheet state="visible" name="sample" sheetId="7" r:id="rId9"/>
+    <sheet name="sheetColumnCount" sheetId="1" r:id="rId1"/>
+    <sheet name="ontology" sheetId="2" r:id="rId2"/>
+    <sheet name="submission" sheetId="3" r:id="rId3"/>
+    <sheet name="contact" sheetId="4" r:id="rId4"/>
+    <sheet name="breed" sheetId="5" r:id="rId5"/>
+    <sheet name="animal" sheetId="6" r:id="rId6"/>
+    <sheet name="sample" sheetId="7" r:id="rId7"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataSignature="AMtx7mj7u11NUWOAME41pst9Su31qW5V8g=="/>
@@ -22,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="119">
   <si>
     <t>Library name</t>
   </si>
@@ -361,42 +370,82 @@
   </si>
   <si>
     <t>VERCH1539971_2010_RegLomBank_PTPLodi_03.09.2011</t>
+  </si>
+  <si>
+    <t>1 year</t>
+  </si>
+  <si>
+    <t>adult</t>
+  </si>
+  <si>
+    <t>mature</t>
+  </si>
+  <si>
+    <t>7 days</t>
+  </si>
+  <si>
+    <t>frozen, -80 degrees Celsius freezer</t>
+  </si>
+  <si>
+    <t>cryopreservation in liquid nitrogen (dead tissue)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="D/M/YYYY"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="9">
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
-      <sz val="10.0"/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF24292E"/>
       <name val="-apple-system"/>
     </font>
     <font>
       <u/>
+      <sz val="12"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -404,132 +453,407 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="10.56"/>
+    <col min="1" max="26" width="10.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3">
-        <v>11.0</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4">
-        <v>8.0</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5">
-        <v>13.0</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6">
-        <v>19.0</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1"/>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -537,14 +861,14 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" ht="15.75" customHeight="1"/>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:2" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -1530,29 +1854,25 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="10.56"/>
-    <col customWidth="1" min="2" max="2" width="39.78"/>
-    <col customWidth="1" min="3" max="26" width="10.56"/>
+    <col min="1" max="1" width="10.59765625" customWidth="1"/>
+    <col min="2" max="2" width="39.796875" customWidth="1"/>
+    <col min="3" max="26" width="10.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1564,7 +1884,7 @@
       </c>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
@@ -1576,7 +1896,7 @@
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -1588,7 +1908,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
@@ -1600,7 +1920,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
@@ -1612,7 +1932,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>33</v>
       </c>
@@ -1624,7 +1944,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>42</v>
       </c>
@@ -1636,19 +1956,19 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="6"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1"/>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -2635,34 +2955,30 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="B3"/>
-    <hyperlink r:id="rId3" ref="B4"/>
-    <hyperlink r:id="rId4" ref="B5"/>
-    <hyperlink r:id="rId5" ref="B6"/>
-    <hyperlink r:id="rId6" ref="B7"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
   </hyperlinks>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="10.56"/>
+    <col min="1" max="26" width="10.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2682,7 +2998,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -2699,20 +3015,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1"/>
-    <row r="4" ht="15.75" customHeight="1"/>
-    <row r="5" ht="15.75" customHeight="1"/>
-    <row r="6" ht="15.75" customHeight="1"/>
-    <row r="7" ht="15.75" customHeight="1"/>
-    <row r="8" ht="15.75" customHeight="1"/>
-    <row r="9" ht="15.75" customHeight="1"/>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -3698,27 +4014,23 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="10.56"/>
+    <col min="1" max="26" width="10.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -3753,7 +4065,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>49</v>
       </c>
@@ -3782,20 +4094,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1"/>
-    <row r="4" ht="15.75" customHeight="1"/>
-    <row r="5" ht="15.75" customHeight="1"/>
-    <row r="6" ht="15.75" customHeight="1"/>
-    <row r="7" ht="15.75" customHeight="1"/>
-    <row r="8" ht="15.75" customHeight="1"/>
-    <row r="9" ht="15.75" customHeight="1"/>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="3" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="4" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="5" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="6" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="7" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="8" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="9" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:11" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -4782,29 +5094,25 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="I2"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="10.56"/>
+    <col min="1" max="26" width="10.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -4830,7 +5138,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>63</v>
       </c>
@@ -4847,7 +5155,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>67</v>
       </c>
@@ -4864,19 +5172,19 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1"/>
-    <row r="5" ht="15.75" customHeight="1"/>
-    <row r="6" ht="15.75" customHeight="1"/>
-    <row r="7" ht="15.75" customHeight="1"/>
-    <row r="8" ht="15.75" customHeight="1"/>
-    <row r="9" ht="15.75" customHeight="1"/>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -5862,27 +6170,25 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="10.56"/>
+    <col min="1" max="26" width="10.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>72</v>
       </c>
@@ -5923,12 +6229,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:13" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>100</v>
       </c>
       <c r="C2" s="2">
-        <v>855.0</v>
+        <v>855</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>63</v>
@@ -5943,12 +6249,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:13" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>104</v>
       </c>
       <c r="C3" s="2">
-        <v>862.0</v>
+        <v>862</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>63</v>
@@ -5966,12 +6272,18 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:13" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>107</v>
       </c>
       <c r="C4" s="2">
-        <v>1440.0</v>
+        <v>1440</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>104</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>67</v>
@@ -5986,18 +6298,18 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1"/>
-    <row r="6" ht="15.75" customHeight="1"/>
-    <row r="7" ht="15.75" customHeight="1"/>
-    <row r="8" ht="15.75" customHeight="1"/>
-    <row r="9" ht="15.75" customHeight="1"/>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="5" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="6" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="7" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="8" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="9" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -6983,27 +7295,43 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="25" width="10.56"/>
+    <col min="1" max="1" width="48.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.09765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.69921875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.8984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="42.09765625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.59765625" bestFit="1" customWidth="1"/>
+    <col min="19" max="25" width="10.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:18" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>71</v>
       </c>
@@ -7059,18 +7387,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:18" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B2" s="2">
-        <v>1834.0</v>
+        <v>1834</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G2" s="8">
-        <v>36313.0</v>
+        <v>36313</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>20</v>
@@ -7082,12 +7410,12 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:18" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B3" s="2">
-        <v>1835.0</v>
+        <v>1835</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>100</v>
@@ -7096,7 +7424,7 @@
         <v>111</v>
       </c>
       <c r="G3" s="8">
-        <v>36334.0</v>
+        <v>36334</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>103</v>
@@ -7105,18 +7433,18 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:18" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B4" s="2">
-        <v>2302.0</v>
+        <v>2302</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>107</v>
       </c>
       <c r="G4" s="8">
-        <v>40789.0</v>
+        <v>40789</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>20</v>
@@ -7127,19 +7455,37 @@
       <c r="L4" s="2" t="s">
         <v>109</v>
       </c>
+      <c r="M4" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>118</v>
+      </c>
+      <c r="R4" s="11" t="s">
+        <v>116</v>
+      </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1"/>
-    <row r="6" ht="15.75" customHeight="1"/>
-    <row r="7" ht="15.75" customHeight="1"/>
-    <row r="8" ht="15.75" customHeight="1"/>
-    <row r="9" ht="15.75" customHeight="1"/>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="5" spans="1:18" ht="15.75" customHeight="1"/>
+    <row r="6" spans="1:18" ht="15.75" customHeight="1"/>
+    <row r="7" spans="1:18" ht="15.75" customHeight="1"/>
+    <row r="8" spans="1:18" ht="15.75" customHeight="1"/>
+    <row r="9" spans="1:18" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:18" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:18" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:18" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:18" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:18" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:18" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:18" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -8125,9 +8471,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
:bug: fix issue with UID and PK in data import
</commit_message>
<xml_diff>
--- a/django-data/image/common/tests/Image_sample_template_with_example_20190405.xlsx
+++ b/django-data/image/common/tests/Image_sample_template_with_example_20190405.xlsx
@@ -640,7 +640,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="G4 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -724,7 +724,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="G4 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -846,7 +846,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="G4 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -911,7 +911,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="G4 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1006,7 +1006,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="1" sqref="G4 F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1201,10 +1201,10 @@
         <v>86</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>84</v>
@@ -1232,26 +1232,26 @@
   <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R4" activeCellId="0" sqref="R4"/>
+      <selection pane="topLeft" activeCell="R4" activeCellId="1" sqref="G4 R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="48.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="27.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="18.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="21.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="21.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="29.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="42.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="28.59"/>

</xml_diff>